<commit_message>
Updated ITA_grids model - 2025-09-01 21:55
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF2A1545-7A82-4B7F-9676-6938FFD6E9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44599ADF-FFAE-4C96-98F2-2D5385CBEB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9863,7 +9863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2120A05-82F5-479F-B954-942F83022715}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912026F5-1D55-4609-89CE-B06F340955E0}">
   <dimension ref="B2:AI1284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA_grids model - 2025-09-05 21:04
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13477F6E-BA32-4E5E-8FA6-03508FE4F5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC52318A-299A-4BD5-9EDE-C0CD468E9712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8763,7 +8763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29A770E-AB74-484C-AEC0-A9D2A8D46A6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4064E900-BD40-4460-812B-BD1CD4FBEE08}">
   <dimension ref="B2:AI1212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA_grids model - 2025-09-05 21:58
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC52318A-299A-4BD5-9EDE-C0CD468E9712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0592952C-1030-487B-AEA8-3C35C1D4924A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8763,7 +8763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4064E900-BD40-4460-812B-BD1CD4FBEE08}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E9703C-A7C3-4D7F-971F-EF5E7138A309}">
   <dimension ref="B2:AI1212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA_grids model - 2025-09-06 12:08
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3998E13F-A99C-4EFF-86B9-AA454F5A7514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F047DC10-C9B5-43B4-AF13-29EB1C48C693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8791,7 +8791,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A995B5-970B-46D6-8E67-A6635067FABE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23D3CF6-C8E6-4413-9CDB-8B7C4A54E1D5}">
   <dimension ref="B2:AI1212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>